<commit_message>
now fit point clouds with different number of points
</commit_message>
<xml_diff>
--- a/3D_Boids_Render/distanceTraveled_origin.xlsx
+++ b/3D_Boids_Render/distanceTraveled_origin.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10,14 +10,14 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B366215-95D7-4DFD-974D-8F9D7D27ABAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="true"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -53,7 +53,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -61,13 +61,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -382,24 +384,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F93"/>
+  <dimension ref="A1:F114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+    <sheetView tabSelected="true" topLeftCell="A55" workbookViewId="0">
       <selection activeCell="T91" sqref="T91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" customWidth="1"/>
-    <col min="2" max="6" width="4.7109375" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" customWidth="true"/>
+    <col min="2" max="2" width="3.7109375" customWidth="true"/>
+    <col min="3" max="6" width="4.7109375" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1">
-        <v>111.60000000000105</v>
-      </c>
-      <c r="B1">
-        <v>0.2</v>
+    <row r="1">
+      <c r="A1" s="0">
+        <v>173.3999999999987</v>
+      </c>
+      <c r="B1" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C1">
         <v>22.799999999999951</v>
@@ -414,12 +417,12 @@
         <v>22.799999999999951</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2">
-        <v>113.40000000000107</v>
-      </c>
-      <c r="B2">
-        <v>4.0000000000000009</v>
+    <row r="2">
+      <c r="A2" s="0">
+        <v>169.7999999999989</v>
+      </c>
+      <c r="B2" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C2">
         <v>18.999999999999964</v>
@@ -434,12 +437,12 @@
         <v>18.999999999999964</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3">
-        <v>107.80000000000099</v>
-      </c>
-      <c r="B3">
-        <v>3.2000000000000006</v>
+    <row r="3">
+      <c r="A3" s="0">
+        <v>173.19999999999871</v>
+      </c>
+      <c r="B3" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C3">
         <v>18.799999999999965</v>
@@ -454,12 +457,12 @@
         <v>18.999999999999964</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4">
-        <v>113.40000000000107</v>
-      </c>
-      <c r="B4">
-        <v>6.6000000000000032</v>
+    <row r="4">
+      <c r="A4" s="0">
+        <v>163.19999999999928</v>
+      </c>
+      <c r="B4" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C4">
         <v>16.199999999999974</v>
@@ -474,12 +477,12 @@
         <v>16.199999999999974</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5">
-        <v>104.20000000000094</v>
-      </c>
-      <c r="B5">
-        <v>9</v>
+    <row r="5">
+      <c r="A5" s="0">
+        <v>166.3999999999991</v>
+      </c>
+      <c r="B5" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C5">
         <v>18.799999999999965</v>
@@ -494,12 +497,12 @@
         <v>18.799999999999965</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
-      <c r="A6">
-        <v>113.40000000000107</v>
-      </c>
-      <c r="B6">
-        <v>15.199999999999978</v>
+    <row r="6">
+      <c r="A6" s="0">
+        <v>169.7999999999989</v>
+      </c>
+      <c r="B6" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C6">
         <v>15.999999999999975</v>
@@ -514,12 +517,12 @@
         <v>16.199999999999974</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
-      <c r="A7">
-        <v>100.40000000000089</v>
-      </c>
-      <c r="B7">
-        <v>6.0000000000000027</v>
+    <row r="7">
+      <c r="A7" s="0">
+        <v>173.19999999999871</v>
+      </c>
+      <c r="B7" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C7">
         <v>15.999999999999975</v>
@@ -534,12 +537,12 @@
         <v>15.999999999999975</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
-      <c r="A8">
-        <v>102.20000000000091</v>
-      </c>
-      <c r="B8">
-        <v>11.999999999999989</v>
+    <row r="8">
+      <c r="A8" s="0">
+        <v>156.39999999999966</v>
+      </c>
+      <c r="B8" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C8">
         <v>21.799999999999955</v>
@@ -554,12 +557,12 @@
         <v>21.799999999999955</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
-      <c r="A9">
-        <v>111.60000000000105</v>
-      </c>
-      <c r="B9">
-        <v>0.2</v>
+    <row r="9">
+      <c r="A9" s="0">
+        <v>159.59999999999948</v>
+      </c>
+      <c r="B9" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C9">
         <v>21.799999999999955</v>
@@ -574,12 +577,12 @@
         <v>21.799999999999955</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
-      <c r="A10">
-        <v>92.000000000000767</v>
-      </c>
-      <c r="B10">
-        <v>11.999999999999989</v>
+    <row r="10">
+      <c r="A10" s="0">
+        <v>162.99999999999929</v>
+      </c>
+      <c r="B10" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C10">
         <v>42.20000000000006</v>
@@ -594,12 +597,12 @@
         <v>42.20000000000006</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
-      <c r="A11">
-        <v>98.400000000000858</v>
-      </c>
-      <c r="B11">
-        <v>17.999999999999968</v>
+    <row r="11">
+      <c r="A11" s="0">
+        <v>166.3999999999991</v>
+      </c>
+      <c r="B11" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C11">
         <v>26.999999999999936</v>
@@ -614,12 +617,12 @@
         <v>26.999999999999936</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
-      <c r="A12">
-        <v>109.80000000000102</v>
-      </c>
-      <c r="B12">
-        <v>3.0000000000000004</v>
+    <row r="12">
+      <c r="A12" s="0">
+        <v>169.7999999999989</v>
+      </c>
+      <c r="B12" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C12">
         <v>42.20000000000006</v>
@@ -634,12 +637,12 @@
         <v>42.20000000000006</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
-      <c r="A13">
-        <v>90.000000000000739</v>
-      </c>
-      <c r="B13">
-        <v>11.999999999999989</v>
+    <row r="13">
+      <c r="A13" s="0">
+        <v>173.3999999999987</v>
+      </c>
+      <c r="B13" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C13">
         <v>17.999999999999968</v>
@@ -654,12 +657,12 @@
         <v>17.999999999999968</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
-      <c r="A14">
-        <v>96.600000000000833</v>
-      </c>
-      <c r="B14">
-        <v>20.999999999999957</v>
+    <row r="14">
+      <c r="A14" s="0">
+        <v>149.80000000000004</v>
+      </c>
+      <c r="B14" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C14">
         <v>20.999999999999957</v>
@@ -674,12 +677,12 @@
         <v>20.999999999999957</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
-      <c r="A15">
-        <v>108.200000000001</v>
-      </c>
-      <c r="B15">
-        <v>6.0000000000000027</v>
+    <row r="15">
+      <c r="A15" s="0">
+        <v>152.99999999999986</v>
+      </c>
+      <c r="B15" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C15">
         <v>20.999999999999957</v>
@@ -694,12 +697,12 @@
         <v>20.999999999999957</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
-      <c r="A16">
-        <v>83.800000000000651</v>
-      </c>
-      <c r="B16">
-        <v>20.999999999999957</v>
+    <row r="16">
+      <c r="A16" s="0">
+        <v>170.39999999999887</v>
+      </c>
+      <c r="B16" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C16">
         <v>45.000000000000099</v>
@@ -714,12 +717,12 @@
         <v>44.800000000000097</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
-      <c r="A17">
-        <v>88.000000000000711</v>
-      </c>
-      <c r="B17">
-        <v>35.999999999999972</v>
+    <row r="17">
+      <c r="A17" s="0">
+        <v>173.99999999999866</v>
+      </c>
+      <c r="B17" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C17">
         <v>65.800000000000395</v>
@@ -734,12 +737,12 @@
         <v>65.800000000000395</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
-      <c r="A18">
-        <v>93.000000000000782</v>
-      </c>
-      <c r="B18">
-        <v>4.2000000000000011</v>
+    <row r="18">
+      <c r="A18" s="0">
+        <v>146.40000000000023</v>
+      </c>
+      <c r="B18" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C18">
         <v>6.6000000000000032</v>
@@ -754,12 +757,12 @@
         <v>36.199999999999974</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
-      <c r="A19">
-        <v>106.60000000000097</v>
-      </c>
-      <c r="B19">
-        <v>4.2000000000000011</v>
+    <row r="19">
+      <c r="A19" s="0">
+        <v>170.99999999999883</v>
+      </c>
+      <c r="B19" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C19">
         <v>21.199999999999957</v>
@@ -774,12 +777,12 @@
         <v>33.199999999999932</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
-      <c r="A20">
-        <v>83.200000000000642</v>
-      </c>
-      <c r="B20">
-        <v>15.199999999999978</v>
+    <row r="20">
+      <c r="A20" s="0">
+        <v>174.79999999999862</v>
+      </c>
+      <c r="B20" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C20">
         <v>17.999999999999968</v>
@@ -794,12 +797,12 @@
         <v>17.999999999999968</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
-      <c r="A21">
-        <v>84.600000000000662</v>
-      </c>
-      <c r="B21">
-        <v>15.199999999999978</v>
+    <row r="21">
+      <c r="A21" s="0">
+        <v>143.00000000000043</v>
+      </c>
+      <c r="B21" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C21">
         <v>17.999999999999968</v>
@@ -814,12 +817,12 @@
         <v>17.999999999999968</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
-      <c r="A22">
-        <v>86.200000000000685</v>
-      </c>
-      <c r="B22">
-        <v>29.999999999999925</v>
+    <row r="22">
+      <c r="A22" s="0">
+        <v>168.19999999999899</v>
+      </c>
+      <c r="B22" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C22">
         <v>32.799999999999926</v>
@@ -834,12 +837,12 @@
         <v>33.399999999999935</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
-      <c r="A23">
-        <v>87.800000000000708</v>
-      </c>
-      <c r="B23">
-        <v>6.6000000000000032</v>
+    <row r="23">
+      <c r="A23" s="0">
+        <v>171.99999999999878</v>
+      </c>
+      <c r="B23" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C23">
         <v>5.8000000000000025</v>
@@ -854,12 +857,12 @@
         <v>11.79999999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
-      <c r="A24">
-        <v>91.200000000000756</v>
-      </c>
-      <c r="B24">
-        <v>8.4000000000000021</v>
+    <row r="24">
+      <c r="A24" s="0">
+        <v>139.60000000000062</v>
+      </c>
+      <c r="B24" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C24">
         <v>5.8000000000000025</v>
@@ -874,12 +877,12 @@
         <v>5.8000000000000025</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
-      <c r="A25">
-        <v>105.00000000000095</v>
-      </c>
-      <c r="B25">
-        <v>24.599999999999945</v>
+    <row r="25">
+      <c r="A25" s="0">
+        <v>161.59999999999937</v>
+      </c>
+      <c r="B25" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C25">
         <v>9</v>
@@ -894,12 +897,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
-      <c r="A26">
-        <v>82.800000000000637</v>
-      </c>
-      <c r="B26">
-        <v>12.199999999999989</v>
+    <row r="26">
+      <c r="A26" s="0">
+        <v>165.39999999999915</v>
+      </c>
+      <c r="B26" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C26">
         <v>5.8000000000000025</v>
@@ -914,12 +917,12 @@
         <v>5.8000000000000025</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
-      <c r="A27">
-        <v>86.000000000000682</v>
-      </c>
-      <c r="B27">
-        <v>26.999999999999936</v>
+    <row r="27">
+      <c r="A27" s="0">
+        <v>133.20000000000098</v>
+      </c>
+      <c r="B27" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C27">
         <v>33.79999999999994</v>
@@ -934,12 +937,12 @@
         <v>33.79999999999994</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
-      <c r="A28">
-        <v>87.600000000000705</v>
-      </c>
-      <c r="B28">
-        <v>13.199999999999985</v>
+    <row r="28">
+      <c r="A28" s="0">
+        <v>136.60000000000079</v>
+      </c>
+      <c r="B28" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C28">
         <v>22.599999999999952</v>
@@ -954,12 +957,12 @@
         <v>6.8000000000000034</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
-      <c r="A29">
-        <v>101.4000000000009</v>
-      </c>
-      <c r="B29">
-        <v>30.399999999999924</v>
+    <row r="29">
+      <c r="A29" s="0">
+        <v>158.79999999999953</v>
+      </c>
+      <c r="B29" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C29">
         <v>27.799999999999933</v>
@@ -974,12 +977,12 @@
         <v>26.999999999999936</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
-      <c r="A30">
-        <v>71.600000000000477</v>
-      </c>
-      <c r="B30">
-        <v>57.00000000000027</v>
+    <row r="30">
+      <c r="A30" s="0">
+        <v>117.00000000000112</v>
+      </c>
+      <c r="B30" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C30">
         <v>54.20000000000023</v>
@@ -994,12 +997,12 @@
         <v>54.20000000000023</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
-      <c r="A31">
-        <v>72.400000000000489</v>
-      </c>
-      <c r="B31">
-        <v>15.999999999999975</v>
+    <row r="31">
+      <c r="A31" s="0">
+        <v>120.20000000000117</v>
+      </c>
+      <c r="B31" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C31">
         <v>10.599999999999994</v>
@@ -1014,12 +1017,12 @@
         <v>10.599999999999994</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
-      <c r="A32">
-        <v>73.2000000000005</v>
-      </c>
-      <c r="B32">
-        <v>51.200000000000188</v>
+    <row r="32">
+      <c r="A32" s="0">
+        <v>123.20000000000121</v>
+      </c>
+      <c r="B32" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C32">
         <v>42.600000000000065</v>
@@ -1034,12 +1037,12 @@
         <v>42.800000000000068</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
-      <c r="A33">
-        <v>74.200000000000514</v>
-      </c>
-      <c r="B33">
-        <v>10.599999999999994</v>
+    <row r="33">
+      <c r="A33" s="0">
+        <v>126.60000000000126</v>
+      </c>
+      <c r="B33" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C33">
         <v>32.199999999999918</v>
@@ -1054,12 +1057,12 @@
         <v>32.199999999999918</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
-      <c r="A34">
-        <v>75.400000000000531</v>
-      </c>
-      <c r="B34">
-        <v>11.79999999999999</v>
+    <row r="34">
+      <c r="A34" s="0">
+        <v>130.00000000000117</v>
+      </c>
+      <c r="B34" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C34">
         <v>38.800000000000011</v>
@@ -1074,12 +1077,12 @@
         <v>38.800000000000011</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
-      <c r="A35">
-        <v>81.000000000000611</v>
-      </c>
-      <c r="B35">
-        <v>12.199999999999989</v>
+    <row r="35">
+      <c r="A35" s="0">
+        <v>156.19999999999968</v>
+      </c>
+      <c r="B35" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C35">
         <v>28.199999999999932</v>
@@ -1094,12 +1097,12 @@
         <v>28.199999999999932</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
-      <c r="A36">
-        <v>86.000000000000682</v>
-      </c>
-      <c r="B36">
-        <v>23.999999999999947</v>
+    <row r="36">
+      <c r="A36" s="0">
+        <v>107.80000000000099</v>
+      </c>
+      <c r="B36" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C36">
         <v>14.799999999999979</v>
@@ -1114,12 +1117,12 @@
         <v>14.799999999999979</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
-      <c r="A37">
-        <v>102.00000000000091</v>
-      </c>
-      <c r="B37">
-        <v>47.200000000000131</v>
+    <row r="37">
+      <c r="A37" s="0">
+        <v>110.80000000000103</v>
+      </c>
+      <c r="B37" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C37">
         <v>21.199999999999957</v>
@@ -1134,12 +1137,12 @@
         <v>35.999999999999972</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
-      <c r="A38">
-        <v>68.800000000000438</v>
-      </c>
-      <c r="B38">
-        <v>34.999999999999957</v>
+    <row r="38">
+      <c r="A38" s="0">
+        <v>113.80000000000108</v>
+      </c>
+      <c r="B38" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C38">
         <v>27.999999999999932</v>
@@ -1154,12 +1157,12 @@
         <v>27.999999999999932</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
-      <c r="A39">
-        <v>76.200000000000543</v>
-      </c>
-      <c r="B39">
-        <v>37.799999999999997</v>
+    <row r="39">
+      <c r="A39" s="0">
+        <v>116.80000000000112</v>
+      </c>
+      <c r="B39" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C39">
         <v>47.200000000000131</v>
@@ -1174,12 +1177,12 @@
         <v>47.400000000000134</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
-      <c r="A40">
-        <v>77.600000000000563</v>
-      </c>
-      <c r="B40">
-        <v>17.199999999999971</v>
+    <row r="40">
+      <c r="A40" s="0">
+        <v>153.79999999999981</v>
+      </c>
+      <c r="B40" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C40">
         <v>17.799999999999969</v>
@@ -1194,12 +1197,12 @@
         <v>17.799999999999969</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
-      <c r="A41">
-        <v>79.200000000000585</v>
-      </c>
-      <c r="B41">
-        <v>17.39999999999997</v>
+    <row r="41">
+      <c r="A41" s="0">
+        <v>101.80000000000091</v>
+      </c>
+      <c r="B41" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C41">
         <v>23.399999999999949</v>
@@ -1214,12 +1217,12 @@
         <v>23.399999999999949</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
-      <c r="A42">
-        <v>80.800000000000608</v>
-      </c>
-      <c r="B42">
-        <v>21.199999999999957</v>
+    <row r="42">
+      <c r="A42" s="0">
+        <v>104.40000000000094</v>
+      </c>
+      <c r="B42" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C42">
         <v>23.399999999999949</v>
@@ -1234,12 +1237,12 @@
         <v>23.399999999999949</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
-      <c r="A43">
-        <v>84.400000000000659</v>
-      </c>
-      <c r="B43">
-        <v>23.399999999999949</v>
+    <row r="43">
+      <c r="A43" s="0">
+        <v>147.20000000000019</v>
+      </c>
+      <c r="B43" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C43">
         <v>19.999999999999961</v>
@@ -1254,12 +1257,12 @@
         <v>19.999999999999961</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
-      <c r="A44">
-        <v>103.00000000000092</v>
-      </c>
-      <c r="B44">
-        <v>51.200000000000188</v>
+    <row r="44">
+      <c r="A44" s="0">
+        <v>151.39999999999995</v>
+      </c>
+      <c r="B44" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C44">
         <v>18.199999999999967</v>
@@ -1274,12 +1277,12 @@
         <v>11.79999999999999</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
-      <c r="A45">
-        <v>66.200000000000401</v>
-      </c>
-      <c r="B45">
-        <v>41.600000000000051</v>
+    <row r="45">
+      <c r="A45" s="0">
+        <v>98.400000000000858</v>
+      </c>
+      <c r="B45" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C45">
         <v>23.399999999999949</v>
@@ -1294,12 +1297,12 @@
         <v>23.399999999999949</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
-      <c r="A46">
-        <v>79.200000000000585</v>
-      </c>
-      <c r="B46">
-        <v>21.199999999999957</v>
+    <row r="46">
+      <c r="A46" s="0">
+        <v>145.00000000000031</v>
+      </c>
+      <c r="B46" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C46">
         <v>19.999999999999961</v>
@@ -1314,12 +1317,12 @@
         <v>19.999999999999961</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
-      <c r="A47">
-        <v>84.600000000000662</v>
-      </c>
-      <c r="B47">
-        <v>21.199999999999957</v>
+    <row r="47">
+      <c r="A47" s="0">
+        <v>149.00000000000009</v>
+      </c>
+      <c r="B47" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C47">
         <v>18.199999999999967</v>
@@ -1334,12 +1337,12 @@
         <v>17.999999999999968</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
-      <c r="A48">
-        <v>104.00000000000094</v>
-      </c>
-      <c r="B48">
-        <v>68.200000000000429</v>
+    <row r="48">
+      <c r="A48" s="0">
+        <v>92.400000000000773</v>
+      </c>
+      <c r="B48" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C48">
         <v>57.00000000000027</v>
@@ -1354,12 +1357,12 @@
         <v>57.00000000000027</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
-      <c r="A49">
-        <v>64.400000000000375</v>
-      </c>
-      <c r="B49">
-        <v>15.999999999999975</v>
+    <row r="49">
+      <c r="A49" s="0">
+        <v>95.200000000000813</v>
+      </c>
+      <c r="B49" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C49">
         <v>66.400000000000404</v>
@@ -1374,12 +1377,12 @@
         <v>35.999999999999972</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
-      <c r="A50">
-        <v>79.400000000000588</v>
-      </c>
-      <c r="B50">
-        <v>23.19999999999995</v>
+    <row r="50">
+      <c r="A50" s="0">
+        <v>104.40000000000094</v>
+      </c>
+      <c r="B50" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C50">
         <v>21.599999999999955</v>
@@ -1394,12 +1397,12 @@
         <v>21.599999999999955</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
-      <c r="A51">
-        <v>85.200000000000671</v>
-      </c>
-      <c r="B51">
-        <v>15.999999999999975</v>
+    <row r="51">
+      <c r="A51" s="0">
+        <v>107.80000000000099</v>
+      </c>
+      <c r="B51" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C51">
         <v>29.799999999999926</v>
@@ -1414,12 +1417,12 @@
         <v>29.799999999999926</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
-      <c r="A52">
-        <v>102.80000000000092</v>
-      </c>
-      <c r="B52">
-        <v>25.599999999999941</v>
+    <row r="52">
+      <c r="A52" s="0">
+        <v>111.40000000000104</v>
+      </c>
+      <c r="B52" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C52">
         <v>29.399999999999928</v>
@@ -1434,12 +1437,12 @@
         <v>29.399999999999928</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
-      <c r="A53">
-        <v>63.400000000000361</v>
-      </c>
-      <c r="B53">
-        <v>55.200000000000244</v>
+    <row r="53">
+      <c r="A53" s="0">
+        <v>142.80000000000044</v>
+      </c>
+      <c r="B53" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C53">
         <v>18.799999999999965</v>
@@ -1454,12 +1457,12 @@
         <v>18.799999999999965</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
-      <c r="A54">
-        <v>78.000000000000568</v>
-      </c>
-      <c r="B54">
-        <v>35.999999999999972</v>
+    <row r="54">
+      <c r="A54" s="0">
+        <v>89.200000000000728</v>
+      </c>
+      <c r="B54" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C54">
         <v>69.000000000000441</v>
@@ -1474,12 +1477,12 @@
         <v>69.000000000000441</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
-      <c r="A55">
-        <v>83.800000000000651</v>
-      </c>
-      <c r="B55">
-        <v>30.599999999999923</v>
+    <row r="55">
+      <c r="A55" s="0">
+        <v>108.80000000000101</v>
+      </c>
+      <c r="B55" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C55">
         <v>21.599999999999955</v>
@@ -1494,12 +1497,12 @@
         <v>21.599999999999955</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
-      <c r="A56">
-        <v>101.6000000000009</v>
-      </c>
-      <c r="B56">
-        <v>33.199999999999932</v>
+    <row r="56">
+      <c r="A56" s="0">
+        <v>112.60000000000106</v>
+      </c>
+      <c r="B56" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C56">
         <v>29.999999999999925</v>
@@ -1514,12 +1517,12 @@
         <v>29.999999999999925</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
-      <c r="A57">
-        <v>61.600000000000335</v>
-      </c>
-      <c r="B57">
-        <v>40.80000000000004</v>
+    <row r="57">
+      <c r="A57" s="0">
+        <v>136.60000000000079</v>
+      </c>
+      <c r="B57" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C57">
         <v>23.399999999999949</v>
@@ -1534,12 +1537,12 @@
         <v>23.399999999999949</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
-      <c r="A58">
-        <v>78.600000000000577</v>
-      </c>
-      <c r="B58">
-        <v>13.399999999999984</v>
+    <row r="58">
+      <c r="A58" s="0">
+        <v>140.80000000000055</v>
+      </c>
+      <c r="B58" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C58">
         <v>21.399999999999956</v>
@@ -1554,12 +1557,12 @@
         <v>21.399999999999956</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
-      <c r="A59">
-        <v>84.600000000000662</v>
-      </c>
-      <c r="B59">
-        <v>11.79999999999999</v>
+    <row r="59">
+      <c r="A59" s="0">
+        <v>86.200000000000685</v>
+      </c>
+      <c r="B59" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C59">
         <v>27.399999999999935</v>
@@ -1574,12 +1577,12 @@
         <v>27.599999999999934</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
-      <c r="A60">
-        <v>98.200000000000855</v>
-      </c>
-      <c r="B60">
-        <v>14.799999999999979</v>
+    <row r="60">
+      <c r="A60" s="0">
+        <v>110.20000000000103</v>
+      </c>
+      <c r="B60" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C60">
         <v>53.000000000000213</v>
@@ -1594,12 +1597,12 @@
         <v>53.200000000000216</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
-      <c r="A61">
-        <v>61.000000000000327</v>
-      </c>
-      <c r="B61">
-        <v>13.399999999999984</v>
+    <row r="61">
+      <c r="A61" s="0">
+        <v>122.00000000000119</v>
+      </c>
+      <c r="B61" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C61">
         <v>19.999999999999961</v>
@@ -1614,12 +1617,12 @@
         <v>19.999999999999961</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
-      <c r="A62">
-        <v>61.800000000000338</v>
-      </c>
-      <c r="B62">
-        <v>14.799999999999979</v>
+    <row r="62">
+      <c r="A62" s="0">
+        <v>134.6000000000009</v>
+      </c>
+      <c r="B62" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C62">
         <v>17.999999999999968</v>
@@ -1634,12 +1637,12 @@
         <v>18.199999999999967</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
-      <c r="A63">
-        <v>63.000000000000355</v>
-      </c>
-      <c r="B63">
-        <v>38</v>
+    <row r="63">
+      <c r="A63" s="0">
+        <v>83.400000000000645</v>
+      </c>
+      <c r="B63" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C63">
         <v>19.999999999999961</v>
@@ -1654,12 +1657,12 @@
         <v>19.999999999999961</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
-      <c r="A64">
-        <v>79.400000000000588</v>
-      </c>
-      <c r="B64">
-        <v>21.599999999999955</v>
+    <row r="64">
+      <c r="A64" s="0">
+        <v>108.00000000000099</v>
+      </c>
+      <c r="B64" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C64">
         <v>21.999999999999954</v>
@@ -1674,12 +1677,12 @@
         <v>21.999999999999954</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
-      <c r="A65">
-        <v>83.600000000000648</v>
-      </c>
-      <c r="B65">
-        <v>50.200000000000173</v>
+    <row r="65">
+      <c r="A65" s="0">
+        <v>120.20000000000117</v>
+      </c>
+      <c r="B65" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C65">
         <v>72.000000000000483</v>
@@ -1694,12 +1697,12 @@
         <v>72.000000000000483</v>
       </c>
     </row>
-    <row r="66" spans="1:6">
-      <c r="A66">
-        <v>85.800000000000679</v>
-      </c>
-      <c r="B66">
-        <v>50.200000000000173</v>
+    <row r="66">
+      <c r="A66" s="0">
+        <v>132.80000000000101</v>
+      </c>
+      <c r="B66" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C66">
         <v>18.799999999999965</v>
@@ -1714,12 +1717,12 @@
         <v>39.200000000000017</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
-      <c r="A67">
-        <v>95.00000000000081</v>
-      </c>
-      <c r="B67">
-        <v>47.400000000000134</v>
+    <row r="67">
+      <c r="A67" s="0">
+        <v>68.400000000000432</v>
+      </c>
+      <c r="B67" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C67">
         <v>18.799999999999965</v>
@@ -1734,12 +1737,12 @@
         <v>18.799999999999965</v>
       </c>
     </row>
-    <row r="68" spans="1:6">
-      <c r="A68">
-        <v>97.200000000000841</v>
-      </c>
-      <c r="B68">
-        <v>23.19999999999995</v>
+    <row r="68">
+      <c r="A68" s="0">
+        <v>70.40000000000046</v>
+      </c>
+      <c r="B68" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C68">
         <v>37.599999999999994</v>
@@ -1754,12 +1757,12 @@
         <v>37.599999999999994</v>
       </c>
     </row>
-    <row r="69" spans="1:6">
-      <c r="A69">
-        <v>62.800000000000352</v>
-      </c>
-      <c r="B69">
-        <v>38</v>
+    <row r="69">
+      <c r="A69" s="0">
+        <v>72.600000000000492</v>
+      </c>
+      <c r="B69" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C69">
         <v>18.799999999999965</v>
@@ -1774,12 +1777,12 @@
         <v>18.799999999999965</v>
       </c>
     </row>
-    <row r="70" spans="1:6">
-      <c r="A70">
-        <v>64.200000000000372</v>
-      </c>
-      <c r="B70">
-        <v>43.60000000000008</v>
+    <row r="70">
+      <c r="A70" s="0">
+        <v>80.800000000000608</v>
+      </c>
+      <c r="B70" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C70">
         <v>18.799999999999965</v>
@@ -1794,12 +1797,12 @@
         <v>23.999999999999947</v>
       </c>
     </row>
-    <row r="71" spans="1:6">
-      <c r="A71">
-        <v>78.200000000000571</v>
-      </c>
-      <c r="B71">
-        <v>41.600000000000051</v>
+    <row r="71">
+      <c r="A71" s="0">
+        <v>106.00000000000097</v>
+      </c>
+      <c r="B71" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C71">
         <v>21.599999999999955</v>
@@ -1814,12 +1817,12 @@
         <v>21.399999999999956</v>
       </c>
     </row>
-    <row r="72" spans="1:6">
-      <c r="A72">
-        <v>84.800000000000665</v>
-      </c>
-      <c r="B72">
-        <v>47.400000000000134</v>
+    <row r="72">
+      <c r="A72" s="0">
+        <v>118.40000000000114</v>
+      </c>
+      <c r="B72" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C72">
         <v>54.000000000000227</v>
@@ -1834,12 +1837,12 @@
         <v>54.000000000000227</v>
       </c>
     </row>
-    <row r="73" spans="1:6">
-      <c r="A73">
-        <v>87.000000000000696</v>
-      </c>
-      <c r="B73">
-        <v>47.200000000000131</v>
+    <row r="73">
+      <c r="A73" s="0">
+        <v>131.2000000000011</v>
+      </c>
+      <c r="B73" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C73">
         <v>53.800000000000225</v>
@@ -1854,12 +1857,12 @@
         <v>54.000000000000227</v>
       </c>
     </row>
-    <row r="74" spans="1:6">
-      <c r="A74">
-        <v>89.200000000000728</v>
-      </c>
-      <c r="B74">
-        <v>47.200000000000131</v>
+    <row r="74">
+      <c r="A74" s="0">
+        <v>63.800000000000367</v>
+      </c>
+      <c r="B74" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C74">
         <v>54.000000000000227</v>
@@ -1874,12 +1877,12 @@
         <v>53.800000000000225</v>
       </c>
     </row>
-    <row r="75" spans="1:6">
-      <c r="A75">
-        <v>91.600000000000762</v>
-      </c>
-      <c r="B75">
-        <v>47.200000000000131</v>
+    <row r="75">
+      <c r="A75" s="0">
+        <v>65.600000000000392</v>
+      </c>
+      <c r="B75" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C75">
         <v>14.799999999999979</v>
@@ -1894,12 +1897,12 @@
         <v>35.999999999999972</v>
       </c>
     </row>
-    <row r="76" spans="1:6">
-      <c r="A76">
-        <v>63.000000000000355</v>
-      </c>
-      <c r="B76">
-        <v>11.79999999999999</v>
+    <row r="76">
+      <c r="A76" s="0">
+        <v>78.400000000000574</v>
+      </c>
+      <c r="B76" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C76">
         <v>23.19999999999995</v>
@@ -1914,12 +1917,12 @@
         <v>22.99999999999995</v>
       </c>
     </row>
-    <row r="77" spans="1:6">
-      <c r="A77">
-        <v>77.40000000000056</v>
-      </c>
-      <c r="B77">
-        <v>23.999999999999947</v>
+    <row r="77">
+      <c r="A77" s="0">
+        <v>104.20000000000094</v>
+      </c>
+      <c r="B77" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C77">
         <v>12.199999999999989</v>
@@ -1934,12 +1937,12 @@
         <v>12.199999999999989</v>
       </c>
     </row>
-    <row r="78" spans="1:6">
-      <c r="A78">
-        <v>79.400000000000588</v>
-      </c>
-      <c r="B78">
-        <v>23.999999999999947</v>
+    <row r="78">
+      <c r="A78" s="0">
+        <v>108.400000000001</v>
+      </c>
+      <c r="B78" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C78">
         <v>29.399999999999928</v>
@@ -1954,12 +1957,12 @@
         <v>29.399999999999928</v>
       </c>
     </row>
-    <row r="79" spans="1:6">
-      <c r="A79">
-        <v>81.60000000000062</v>
-      </c>
-      <c r="B79">
-        <v>23.999999999999947</v>
+    <row r="79">
+      <c r="A79" s="0">
+        <v>112.60000000000106</v>
+      </c>
+      <c r="B79" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C79">
         <v>29.399999999999928</v>
@@ -1974,12 +1977,12 @@
         <v>29.399999999999928</v>
       </c>
     </row>
-    <row r="80" spans="1:6">
-      <c r="A80">
-        <v>83.800000000000651</v>
-      </c>
-      <c r="B80">
-        <v>23.999999999999947</v>
+    <row r="80">
+      <c r="A80" s="0">
+        <v>116.80000000000112</v>
+      </c>
+      <c r="B80" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C80">
         <v>12.599999999999987</v>
@@ -1994,12 +1997,12 @@
         <v>12.599999999999987</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
-      <c r="A81">
-        <v>63.400000000000361</v>
-      </c>
-      <c r="B81">
-        <v>14.999999999999979</v>
+    <row r="81">
+      <c r="A81" s="0">
+        <v>129.80000000000118</v>
+      </c>
+      <c r="B81" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C81">
         <v>12.599999999999987</v>
@@ -2014,12 +2017,12 @@
         <v>12.399999999999988</v>
       </c>
     </row>
-    <row r="82" spans="1:6">
-      <c r="A82">
-        <v>76.400000000000546</v>
-      </c>
-      <c r="B82">
-        <v>10.599999999999994</v>
+    <row r="82">
+      <c r="A82" s="0">
+        <v>134.20000000000093</v>
+      </c>
+      <c r="B82" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C82">
         <v>12.599999999999987</v>
@@ -2034,12 +2037,12 @@
         <v>12.599999999999987</v>
       </c>
     </row>
-    <row r="83" spans="1:6">
-      <c r="A83">
-        <v>62.400000000000347</v>
-      </c>
-      <c r="B83">
-        <v>18.999999999999964</v>
+    <row r="83">
+      <c r="A83" s="0">
+        <v>61.20000000000033</v>
+      </c>
+      <c r="B83" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C83">
         <v>12.599999999999987</v>
@@ -2054,12 +2057,12 @@
         <v>12.599999999999987</v>
       </c>
     </row>
-    <row r="84" spans="1:6">
-      <c r="A84">
-        <v>73.600000000000506</v>
-      </c>
-      <c r="B84">
-        <v>6.6000000000000032</v>
+    <row r="84">
+      <c r="A84" s="0">
+        <v>76.400000000000546</v>
+      </c>
+      <c r="B84" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C84">
         <v>12.599999999999987</v>
@@ -2074,12 +2077,12 @@
         <v>12.399999999999988</v>
       </c>
     </row>
-    <row r="85" spans="1:6">
-      <c r="A85">
-        <v>63.400000000000361</v>
-      </c>
-      <c r="B85">
-        <v>21.199999999999957</v>
+    <row r="85">
+      <c r="A85" s="0">
+        <v>111.00000000000104</v>
+      </c>
+      <c r="B85" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C85">
         <v>12.599999999999987</v>
@@ -2094,12 +2097,12 @@
         <v>12.399999999999988</v>
       </c>
     </row>
-    <row r="86" spans="1:6">
-      <c r="A86">
-        <v>70.800000000000466</v>
-      </c>
-      <c r="B86">
-        <v>12.399999999999988</v>
+    <row r="86">
+      <c r="A86" s="0">
+        <v>115.4000000000011</v>
+      </c>
+      <c r="B86" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C86">
         <v>28.59999999999993</v>
@@ -2114,12 +2117,12 @@
         <v>28.59999999999993</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
-      <c r="A87">
-        <v>72.800000000000495</v>
-      </c>
-      <c r="B87">
-        <v>12.399999999999988</v>
+    <row r="87">
+      <c r="A87" s="0">
+        <v>133.00000000000099</v>
+      </c>
+      <c r="B87" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C87">
         <v>12.599999999999987</v>
@@ -2134,12 +2137,12 @@
         <v>12.399999999999988</v>
       </c>
     </row>
-    <row r="88" spans="1:6">
-      <c r="A88">
-        <v>64.400000000000375</v>
-      </c>
-      <c r="B88">
-        <v>14.999999999999979</v>
+    <row r="88">
+      <c r="A88" s="0">
+        <v>59.000000000000298</v>
+      </c>
+      <c r="B88" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C88">
         <v>14.999999999999979</v>
@@ -2154,12 +2157,12 @@
         <v>14.999999999999979</v>
       </c>
     </row>
-    <row r="89" spans="1:6">
-      <c r="A89">
-        <v>66.200000000000401</v>
-      </c>
-      <c r="B89">
-        <v>11.999999999999989</v>
+    <row r="89">
+      <c r="A89" s="0">
+        <v>60.800000000000324</v>
+      </c>
+      <c r="B89" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C89">
         <v>11.999999999999989</v>
@@ -2174,12 +2177,12 @@
         <v>11.999999999999989</v>
       </c>
     </row>
-    <row r="90" spans="1:6">
-      <c r="A90">
-        <v>68.200000000000429</v>
-      </c>
-      <c r="B90">
-        <v>9</v>
+    <row r="90">
+      <c r="A90" s="0">
+        <v>74.60000000000052</v>
+      </c>
+      <c r="B90" s="0">
+        <v>0.20000000000000001</v>
       </c>
       <c r="C90">
         <v>9</v>
@@ -2194,10 +2197,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91">
+      <c r="A91" s="0">
+        <v>114.20000000000108</v>
+      </c>
       <c r="B91" s="1">
-        <f>AVERAGE(B1:B90)</f>
-        <v>23.228888888888903</v>
+        <v>0.20000000000000001</v>
       </c>
       <c r="C91" s="1">
         <f t="shared" ref="C91:F91" si="0">AVERAGE(C1:C90)</f>
@@ -2216,10 +2221,12 @@
         <v>26.420000000000009</v>
       </c>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92">
+      <c r="A92" s="0">
+        <v>118.60000000000115</v>
+      </c>
       <c r="B92" s="1">
-        <f>MIN(B1:B90)</f>
-        <v>0.2</v>
+        <v>0.20000000000000001</v>
       </c>
       <c r="C92" s="1">
         <f t="shared" ref="C92:F92" si="1">MIN(C1:C90)</f>
@@ -2238,10 +2245,12 @@
         <v>5.8000000000000025</v>
       </c>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93">
+      <c r="A93" s="0">
+        <v>132.00000000000105</v>
+      </c>
       <c r="B93" s="1">
-        <f>MAX(B1:B90)</f>
-        <v>68.200000000000429</v>
+        <v>0.20000000000000001</v>
       </c>
       <c r="C93" s="1">
         <f t="shared" ref="C93:F93" si="2">MAX(C1:C90)</f>
@@ -2258,6 +2267,174 @@
       <c r="F93" s="1">
         <f t="shared" si="2"/>
         <v>72.000000000000483</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="0">
+        <v>136.60000000000079</v>
+      </c>
+      <c r="B94" s="0">
+        <v>0.20000000000000001</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="0">
+        <v>59.000000000000298</v>
+      </c>
+      <c r="B95" s="0">
+        <v>0.20000000000000001</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="0">
+        <v>61.20000000000033</v>
+      </c>
+      <c r="B96" s="0">
+        <v>0.20000000000000001</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="0">
+        <v>63.800000000000367</v>
+      </c>
+      <c r="B97" s="0">
+        <v>0.20000000000000001</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="0">
+        <v>66.600000000000406</v>
+      </c>
+      <c r="B98" s="0">
+        <v>0.20000000000000001</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="0">
+        <v>69.800000000000452</v>
+      </c>
+      <c r="B99" s="0">
+        <v>0.20000000000000001</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="0">
+        <v>73.000000000000497</v>
+      </c>
+      <c r="B100" s="0">
+        <v>0.20000000000000001</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="0">
+        <v>76.600000000000549</v>
+      </c>
+      <c r="B101" s="0">
+        <v>0.20000000000000001</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="0">
+        <v>80.2000000000006</v>
+      </c>
+      <c r="B102" s="0">
+        <v>0.20000000000000001</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="0">
+        <v>84.000000000000654</v>
+      </c>
+      <c r="B103" s="0">
+        <v>0.20000000000000001</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="0">
+        <v>88.000000000000711</v>
+      </c>
+      <c r="B104" s="0">
+        <v>0.20000000000000001</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="0">
+        <v>92.000000000000767</v>
+      </c>
+      <c r="B105" s="0">
+        <v>0.20000000000000001</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="0">
+        <v>96.000000000000824</v>
+      </c>
+      <c r="B106" s="0">
+        <v>0.20000000000000001</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="0">
+        <v>100.20000000000088</v>
+      </c>
+      <c r="B107" s="0">
+        <v>0.20000000000000001</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="0">
+        <v>104.40000000000094</v>
+      </c>
+      <c r="B108" s="0">
+        <v>0.20000000000000001</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="0">
+        <v>108.80000000000101</v>
+      </c>
+      <c r="B109" s="0">
+        <v>0.20000000000000001</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="0">
+        <v>113.20000000000107</v>
+      </c>
+      <c r="B110" s="0">
+        <v>0.20000000000000001</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="0">
+        <v>117.60000000000113</v>
+      </c>
+      <c r="B111" s="0">
+        <v>0.20000000000000001</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="0">
+        <v>122.00000000000119</v>
+      </c>
+      <c r="B112" s="0">
+        <v>0.20000000000000001</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="0">
+        <v>126.60000000000126</v>
+      </c>
+      <c r="B113" s="0">
+        <v>0.20000000000000001</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="0">
+        <v>131.2000000000011</v>
+      </c>
+      <c r="B114" s="0">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2275,11 +2452,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" customWidth="1"/>
-    <col min="2" max="6" width="4.7109375" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" customWidth="true"/>
+    <col min="2" max="6" width="4.7109375" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1">
       <c r="A1">
         <v>111.60000000000105</v>
       </c>
@@ -2299,7 +2476,7 @@
         <v>22.799999999999951</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2">
       <c r="A2">
         <v>113.40000000000107</v>
       </c>
@@ -2319,7 +2496,7 @@
         <v>18.999999999999964</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3">
       <c r="A3">
         <v>107.80000000000099</v>
       </c>
@@ -2339,7 +2516,7 @@
         <v>18.799999999999965</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4">
       <c r="A4">
         <v>113.20000000000107</v>
       </c>
@@ -2359,7 +2536,7 @@
         <v>16.199999999999974</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5">
       <c r="A5">
         <v>104.00000000000094</v>
       </c>
@@ -2379,7 +2556,7 @@
         <v>18.599999999999966</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6">
       <c r="A6">
         <v>113.40000000000107</v>
       </c>
@@ -2399,7 +2576,7 @@
         <v>16.199999999999974</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7">
       <c r="A7">
         <v>100.40000000000089</v>
       </c>
@@ -2419,7 +2596,7 @@
         <v>46.000000000000114</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8">
       <c r="A8">
         <v>102.20000000000091</v>
       </c>
@@ -2439,7 +2616,7 @@
         <v>21.599999999999955</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9">
       <c r="A9">
         <v>111.60000000000105</v>
       </c>
@@ -2459,7 +2636,7 @@
         <v>21.799999999999955</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10">
       <c r="A10">
         <v>92.000000000000767</v>
       </c>
@@ -2479,7 +2656,7 @@
         <v>42.000000000000057</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11">
       <c r="A11">
         <v>98.400000000000858</v>
       </c>
@@ -2499,7 +2676,7 @@
         <v>26.799999999999937</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12">
       <c r="A12">
         <v>109.80000000000102</v>
       </c>
@@ -2519,7 +2696,7 @@
         <v>42.20000000000006</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13">
       <c r="A13">
         <v>90.000000000000739</v>
       </c>
@@ -2539,7 +2716,7 @@
         <v>17.999999999999968</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14">
       <c r="A14">
         <v>96.600000000000833</v>
       </c>
@@ -2559,7 +2736,7 @@
         <v>20.799999999999958</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15">
       <c r="A15">
         <v>108.200000000001</v>
       </c>
@@ -2579,7 +2756,7 @@
         <v>20.999999999999957</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16">
       <c r="A16">
         <v>83.800000000000651</v>
       </c>
@@ -2599,7 +2776,7 @@
         <v>44.800000000000097</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17">
       <c r="A17">
         <v>88.000000000000711</v>
       </c>
@@ -2619,7 +2796,7 @@
         <v>65.800000000000395</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18">
       <c r="A18">
         <v>93.000000000000782</v>
       </c>
@@ -2639,7 +2816,7 @@
         <v>6.400000000000003</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19">
       <c r="A19">
         <v>106.40000000000097</v>
       </c>
@@ -2659,7 +2836,7 @@
         <v>20.799999999999958</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20">
       <c r="A20">
         <v>83.200000000000642</v>
       </c>
@@ -2679,7 +2856,7 @@
         <v>17.999999999999968</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21">
       <c r="A21">
         <v>84.600000000000662</v>
       </c>
@@ -2699,7 +2876,7 @@
         <v>17.999999999999968</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22">
       <c r="A22">
         <v>86.200000000000685</v>
       </c>
@@ -2719,7 +2896,7 @@
         <v>32.799999999999926</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23">
       <c r="A23">
         <v>87.800000000000708</v>
       </c>
@@ -2739,7 +2916,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24">
       <c r="A24">
         <v>91.200000000000756</v>
       </c>
@@ -2759,7 +2936,7 @@
         <v>17.599999999999969</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25">
       <c r="A25">
         <v>105.00000000000095</v>
       </c>
@@ -2779,7 +2956,7 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26">
       <c r="A26">
         <v>82.800000000000637</v>
       </c>
@@ -2799,7 +2976,7 @@
         <v>8.6000000000000014</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27">
       <c r="A27">
         <v>86.000000000000682</v>
       </c>
@@ -2819,7 +2996,7 @@
         <v>24.799999999999944</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28">
       <c r="A28">
         <v>87.600000000000705</v>
       </c>
@@ -2839,7 +3016,7 @@
         <v>22.599999999999952</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29">
       <c r="A29">
         <v>101.2000000000009</v>
       </c>
@@ -2859,7 +3036,7 @@
         <v>27.599999999999934</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30">
       <c r="A30">
         <v>71.400000000000475</v>
       </c>
@@ -2879,7 +3056,7 @@
         <v>54.000000000000227</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31">
       <c r="A31">
         <v>72.200000000000486</v>
       </c>
@@ -2899,7 +3076,7 @@
         <v>10.599999999999994</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32">
       <c r="A32">
         <v>73.2000000000005</v>
       </c>
@@ -2919,7 +3096,7 @@
         <v>42.600000000000065</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33">
       <c r="A33">
         <v>74.200000000000514</v>
       </c>
@@ -2939,7 +3116,7 @@
         <v>32.199999999999918</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34">
       <c r="A34">
         <v>75.400000000000531</v>
       </c>
@@ -2959,7 +3136,7 @@
         <v>38.800000000000011</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35">
       <c r="A35">
         <v>80.800000000000608</v>
       </c>
@@ -2979,7 +3156,7 @@
         <v>27.999999999999932</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36">
       <c r="A36">
         <v>86.000000000000682</v>
       </c>
@@ -2999,7 +3176,7 @@
         <v>14.799999999999979</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37">
       <c r="A37">
         <v>102.00000000000091</v>
       </c>
@@ -3019,7 +3196,7 @@
         <v>20.999999999999957</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38">
       <c r="A38">
         <v>68.800000000000438</v>
       </c>
@@ -3039,7 +3216,7 @@
         <v>27.999999999999932</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39">
       <c r="A39">
         <v>76.200000000000543</v>
       </c>
@@ -3059,7 +3236,7 @@
         <v>47.200000000000131</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40">
       <c r="A40">
         <v>77.600000000000563</v>
       </c>
@@ -3079,7 +3256,7 @@
         <v>17.599999999999969</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41">
       <c r="A41">
         <v>79.200000000000585</v>
       </c>
@@ -3099,7 +3276,7 @@
         <v>23.19999999999995</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42">
       <c r="A42">
         <v>80.800000000000608</v>
       </c>
@@ -3119,7 +3296,7 @@
         <v>23.19999999999995</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43">
       <c r="A43">
         <v>84.200000000000657</v>
       </c>
@@ -3139,7 +3316,7 @@
         <v>19.999999999999961</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44">
       <c r="A44">
         <v>102.80000000000092</v>
       </c>
@@ -3159,7 +3336,7 @@
         <v>17.999999999999968</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45">
       <c r="A45">
         <v>66.200000000000401</v>
       </c>
@@ -3179,7 +3356,7 @@
         <v>23.399999999999949</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46">
       <c r="A46">
         <v>79.200000000000585</v>
       </c>
@@ -3199,7 +3376,7 @@
         <v>19.999999999999961</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47">
       <c r="A47">
         <v>84.600000000000662</v>
       </c>
@@ -3219,7 +3396,7 @@
         <v>17.999999999999968</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48">
       <c r="A48">
         <v>103.80000000000094</v>
       </c>
@@ -3239,7 +3416,7 @@
         <v>56.800000000000267</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49">
       <c r="A49">
         <v>64.400000000000375</v>
       </c>
@@ -3259,7 +3436,7 @@
         <v>66.200000000000401</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50">
       <c r="A50">
         <v>79.400000000000588</v>
       </c>
@@ -3279,7 +3456,7 @@
         <v>21.399999999999956</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51">
       <c r="A51">
         <v>85.200000000000671</v>
       </c>
@@ -3299,7 +3476,7 @@
         <v>29.799999999999926</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52">
       <c r="A52">
         <v>102.80000000000092</v>
       </c>
@@ -3319,7 +3496,7 @@
         <v>29.199999999999928</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53">
       <c r="A53">
         <v>63.200000000000358</v>
       </c>
@@ -3339,7 +3516,7 @@
         <v>18.799999999999965</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54">
       <c r="A54">
         <v>78.000000000000568</v>
       </c>
@@ -3359,7 +3536,7 @@
         <v>69.000000000000441</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55">
       <c r="A55">
         <v>83.800000000000651</v>
       </c>
@@ -3379,7 +3556,7 @@
         <v>21.399999999999956</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56">
       <c r="A56">
         <v>101.6000000000009</v>
       </c>
@@ -3399,7 +3576,7 @@
         <v>29.999999999999925</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57">
       <c r="A57">
         <v>61.600000000000335</v>
       </c>
@@ -3419,7 +3596,7 @@
         <v>23.399999999999949</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58">
       <c r="A58">
         <v>78.600000000000577</v>
       </c>
@@ -3439,7 +3616,7 @@
         <v>25.199999999999942</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59">
       <c r="A59">
         <v>84.600000000000662</v>
       </c>
@@ -3459,7 +3636,7 @@
         <v>27.399999999999935</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60">
       <c r="A60">
         <v>98.200000000000855</v>
       </c>
@@ -3479,7 +3656,7 @@
         <v>53.000000000000213</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61">
       <c r="A61">
         <v>60.800000000000324</v>
       </c>
@@ -3499,7 +3676,7 @@
         <v>19.799999999999962</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62">
       <c r="A62">
         <v>61.800000000000338</v>
       </c>
@@ -3519,7 +3696,7 @@
         <v>17.799999999999969</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63">
       <c r="A63">
         <v>63.000000000000355</v>
       </c>
@@ -3539,7 +3716,7 @@
         <v>19.999999999999961</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64">
       <c r="A64">
         <v>79.400000000000588</v>
       </c>
@@ -3559,7 +3736,7 @@
         <v>27.399999999999935</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65">
       <c r="A65">
         <v>83.600000000000648</v>
       </c>
@@ -3579,7 +3756,7 @@
         <v>71.80000000000048</v>
       </c>
     </row>
-    <row r="66" spans="1:6">
+    <row r="66">
       <c r="A66">
         <v>85.600000000000676</v>
       </c>
@@ -3599,7 +3776,7 @@
         <v>39.200000000000017</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67">
       <c r="A67">
         <v>94.800000000000807</v>
       </c>
@@ -3619,7 +3796,7 @@
         <v>18.799999999999965</v>
       </c>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68">
       <c r="A68">
         <v>97.200000000000841</v>
       </c>
@@ -3639,7 +3816,7 @@
         <v>37.599999999999994</v>
       </c>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69">
       <c r="A69">
         <v>62.800000000000352</v>
       </c>
@@ -3659,7 +3836,7 @@
         <v>18.799999999999965</v>
       </c>
     </row>
-    <row r="70" spans="1:6">
+    <row r="70">
       <c r="A70">
         <v>64.200000000000372</v>
       </c>
@@ -3679,7 +3856,7 @@
         <v>18.799999999999965</v>
       </c>
     </row>
-    <row r="71" spans="1:6">
+    <row r="71">
       <c r="A71">
         <v>78.200000000000571</v>
       </c>
@@ -3699,7 +3876,7 @@
         <v>21.399999999999956</v>
       </c>
     </row>
-    <row r="72" spans="1:6">
+    <row r="72">
       <c r="A72">
         <v>84.600000000000662</v>
       </c>
@@ -3719,7 +3896,7 @@
         <v>53.800000000000225</v>
       </c>
     </row>
-    <row r="73" spans="1:6">
+    <row r="73">
       <c r="A73">
         <v>87.000000000000696</v>
       </c>
@@ -3739,7 +3916,7 @@
         <v>53.800000000000225</v>
       </c>
     </row>
-    <row r="74" spans="1:6">
+    <row r="74">
       <c r="A74">
         <v>89.200000000000728</v>
       </c>
@@ -3759,7 +3936,7 @@
         <v>44.400000000000091</v>
       </c>
     </row>
-    <row r="75" spans="1:6">
+    <row r="75">
       <c r="A75">
         <v>91.600000000000762</v>
       </c>
@@ -3779,7 +3956,7 @@
         <v>35.999999999999972</v>
       </c>
     </row>
-    <row r="76" spans="1:6">
+    <row r="76">
       <c r="A76">
         <v>63.000000000000355</v>
       </c>
@@ -3799,7 +3976,7 @@
         <v>22.799999999999951</v>
       </c>
     </row>
-    <row r="77" spans="1:6">
+    <row r="77">
       <c r="A77">
         <v>77.200000000000557</v>
       </c>
@@ -3819,7 +3996,7 @@
         <v>12.199999999999989</v>
       </c>
     </row>
-    <row r="78" spans="1:6">
+    <row r="78">
       <c r="A78">
         <v>79.400000000000588</v>
       </c>
@@ -3839,7 +4016,7 @@
         <v>29.199999999999928</v>
       </c>
     </row>
-    <row r="79" spans="1:6">
+    <row r="79">
       <c r="A79">
         <v>81.60000000000062</v>
       </c>
@@ -3859,7 +4036,7 @@
         <v>29.199999999999928</v>
       </c>
     </row>
-    <row r="80" spans="1:6">
+    <row r="80">
       <c r="A80">
         <v>83.800000000000651</v>
       </c>
@@ -3879,7 +4056,7 @@
         <v>12.599999999999987</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81">
       <c r="A81">
         <v>63.400000000000361</v>
       </c>
@@ -3899,7 +4076,7 @@
         <v>12.399999999999988</v>
       </c>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82">
       <c r="A82">
         <v>76.400000000000546</v>
       </c>
@@ -3919,7 +4096,7 @@
         <v>12.599999999999987</v>
       </c>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83">
       <c r="A83">
         <v>62.400000000000347</v>
       </c>
@@ -3939,7 +4116,7 @@
         <v>12.599999999999987</v>
       </c>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84">
       <c r="A84">
         <v>73.600000000000506</v>
       </c>
@@ -3959,7 +4136,7 @@
         <v>12.399999999999988</v>
       </c>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85">
       <c r="A85">
         <v>63.200000000000358</v>
       </c>
@@ -3979,7 +4156,7 @@
         <v>12.399999999999988</v>
       </c>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86">
       <c r="A86">
         <v>70.800000000000466</v>
       </c>
@@ -3999,7 +4176,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87">
       <c r="A87">
         <v>72.800000000000495</v>
       </c>
@@ -4019,7 +4196,7 @@
         <v>12.399999999999988</v>
       </c>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88">
       <c r="A88">
         <v>64.400000000000375</v>
       </c>
@@ -4039,7 +4216,7 @@
         <v>14.999999999999979</v>
       </c>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89">
       <c r="A89">
         <v>66.200000000000401</v>
       </c>
@@ -4059,7 +4236,7 @@
         <v>11.999999999999989</v>
       </c>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90">
       <c r="A90">
         <v>68.200000000000429</v>
       </c>
@@ -4079,7 +4256,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91">
       <c r="B91" s="1">
         <f>AVERAGE(B1:B90)</f>
         <v>23.171111111111127</v>
@@ -4101,7 +4278,7 @@
         <v>26.637777777777778</v>
       </c>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92">
       <c r="B92" s="1">
         <f>MIN(B1:B90)</f>
         <v>0.2</v>
@@ -4123,7 +4300,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93">
       <c r="B93" s="1">
         <f>MAX(B1:B90)</f>
         <v>68.000000000000426</v>
@@ -4160,11 +4337,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" customWidth="1"/>
-    <col min="2" max="6" width="4.7109375" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" customWidth="true"/>
+    <col min="2" max="6" width="4.7109375" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1">
       <c r="A1">
         <v>63.000000000000355</v>
       </c>
@@ -4184,7 +4361,7 @@
         <v>18.599999999999966</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2">
       <c r="A2">
         <v>98.000000000000853</v>
       </c>
@@ -4204,7 +4381,7 @@
         <v>52.80000000000021</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3">
       <c r="A3">
         <v>79.000000000000583</v>
       </c>
@@ -4224,7 +4401,7 @@
         <v>19.799999999999962</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4">
       <c r="A4">
         <v>61.400000000000333</v>
       </c>
@@ -4244,7 +4421,7 @@
         <v>23.19999999999995</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5">
       <c r="A5">
         <v>101.4000000000009</v>
       </c>
@@ -4264,7 +4441,7 @@
         <v>29.799999999999926</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6">
       <c r="A6">
         <v>66.000000000000398</v>
       </c>
@@ -4284,7 +4461,7 @@
         <v>23.19999999999995</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7">
       <c r="A7">
         <v>94.600000000000804</v>
       </c>
@@ -4304,7 +4481,7 @@
         <v>18.599999999999966</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8">
       <c r="A8">
         <v>102.60000000000092</v>
       </c>
@@ -4324,7 +4501,7 @@
         <v>17.799999999999969</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9">
       <c r="A9">
         <v>97.000000000000838</v>
       </c>
@@ -4344,7 +4521,7 @@
         <v>37.399999999999991</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10">
       <c r="A10">
         <v>63.800000000000367</v>
       </c>
@@ -4364,7 +4541,7 @@
         <v>18.599999999999966</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11">
       <c r="A11">
         <v>62.60000000000035</v>
       </c>
@@ -4384,7 +4561,7 @@
         <v>19.799999999999962</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12">
       <c r="A12">
         <v>62.60000000000035</v>
       </c>
@@ -4404,7 +4581,7 @@
         <v>22.599999999999952</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13">
       <c r="A13">
         <v>85.600000000000676</v>
       </c>
@@ -4424,7 +4601,7 @@
         <v>14.199999999999982</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14">
       <c r="A14">
         <v>62.60000000000035</v>
       </c>
@@ -4444,7 +4621,7 @@
         <v>18.599999999999966</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15">
       <c r="A15">
         <v>100.20000000000088</v>
       </c>
@@ -4464,7 +4641,7 @@
         <v>45.400000000000105</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16">
       <c r="A16">
         <v>85.400000000000674</v>
       </c>
@@ -4484,7 +4661,7 @@
         <v>18.399999999999967</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17">
       <c r="A17">
         <v>109.60000000000102</v>
       </c>
@@ -4504,7 +4681,7 @@
         <v>41.600000000000051</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18">
       <c r="A18">
         <v>83.600000000000648</v>
       </c>
@@ -4524,7 +4701,7 @@
         <v>21.199999999999957</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19">
       <c r="A19">
         <v>62.200000000000344</v>
       </c>
@@ -4544,7 +4721,7 @@
         <v>39.800000000000026</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20">
       <c r="A20">
         <v>101.80000000000091</v>
       </c>
@@ -4564,7 +4741,7 @@
         <v>20.799999999999958</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21">
       <c r="A21">
         <v>91.400000000000759</v>
       </c>
@@ -4584,7 +4761,7 @@
         <v>14.399999999999981</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22">
       <c r="A22">
         <v>64.200000000000372</v>
       </c>
@@ -4604,7 +4781,7 @@
         <v>65.600000000000392</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23">
       <c r="A23">
         <v>74.000000000000512</v>
       </c>
@@ -4624,7 +4801,7 @@
         <v>31.999999999999918</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24">
       <c r="A24">
         <v>75.200000000000529</v>
       </c>
@@ -4644,7 +4821,7 @@
         <v>38.400000000000006</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25">
       <c r="A25">
         <v>77.800000000000566</v>
       </c>
@@ -4664,7 +4841,7 @@
         <v>68.600000000000435</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26">
       <c r="A26">
         <v>106.20000000000097</v>
       </c>
@@ -4684,7 +4861,7 @@
         <v>35.19999999999996</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27">
       <c r="A27">
         <v>113.00000000000107</v>
       </c>
@@ -4704,7 +4881,7 @@
         <v>25.599999999999941</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28">
       <c r="A28">
         <v>63.000000000000355</v>
       </c>
@@ -4724,7 +4901,7 @@
         <v>30.399999999999924</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29">
       <c r="A29">
         <v>113.20000000000107</v>
       </c>
@@ -4744,7 +4921,7 @@
         <v>16.199999999999974</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30">
       <c r="A30">
         <v>91.800000000000765</v>
       </c>
@@ -4764,7 +4941,7 @@
         <v>41.600000000000051</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31">
       <c r="A31">
         <v>83.600000000000648</v>
       </c>
@@ -4784,7 +4961,7 @@
         <v>12.399999999999988</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32">
       <c r="A32">
         <v>84.800000000000665</v>
       </c>
@@ -4804,7 +4981,7 @@
         <v>29.399999999999928</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33">
       <c r="A33">
         <v>79.200000000000585</v>
       </c>
@@ -4824,7 +5001,7 @@
         <v>21.199999999999957</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34">
       <c r="A34">
         <v>87.800000000000708</v>
       </c>
@@ -4844,7 +5021,7 @@
         <v>65.200000000000387</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35">
       <c r="A35">
         <v>87.400000000000702</v>
       </c>
@@ -4864,7 +5041,7 @@
         <v>19.399999999999963</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36">
       <c r="A36">
         <v>78.000000000000568</v>
       </c>
@@ -4884,7 +5061,7 @@
         <v>20.799999999999958</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37">
       <c r="A37">
         <v>101.0000000000009</v>
       </c>
@@ -4904,7 +5081,7 @@
         <v>24.799999999999944</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38">
       <c r="A38">
         <v>84.000000000000654</v>
       </c>
@@ -4924,7 +5101,7 @@
         <v>19.599999999999962</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39">
       <c r="A39">
         <v>80.600000000000605</v>
       </c>
@@ -4944,7 +5121,7 @@
         <v>18.799999999999965</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40">
       <c r="A40">
         <v>80.600000000000605</v>
       </c>
@@ -4964,7 +5141,7 @@
         <v>27.799999999999933</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41">
       <c r="A41">
         <v>84.400000000000659</v>
       </c>
@@ -4984,7 +5161,7 @@
         <v>25.399999999999942</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42">
       <c r="A42">
         <v>89.000000000000725</v>
       </c>
@@ -5004,7 +5181,7 @@
         <v>25.399999999999942</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43">
       <c r="A43">
         <v>86.600000000000691</v>
       </c>
@@ -5024,7 +5201,7 @@
         <v>53.400000000000219</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44">
       <c r="A44">
         <v>78.200000000000571</v>
       </c>
@@ -5044,7 +5221,7 @@
         <v>24.999999999999943</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45">
       <c r="A45">
         <v>104.60000000000095</v>
       </c>
@@ -5064,7 +5241,7 @@
         <v>5.6000000000000023</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46">
       <c r="A46">
         <v>83.600000000000648</v>
       </c>
@@ -5084,7 +5261,7 @@
         <v>44.200000000000088</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47">
       <c r="A47">
         <v>73.2000000000005</v>
       </c>
@@ -5104,7 +5281,7 @@
         <v>22.199999999999953</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48">
       <c r="A48">
         <v>79.000000000000583</v>
       </c>
@@ -5124,7 +5301,7 @@
         <v>22.99999999999995</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49">
       <c r="A49">
         <v>77.000000000000554</v>
       </c>
@@ -5144,7 +5321,7 @@
         <v>11.79999999999999</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50">
       <c r="A50">
         <v>83.200000000000642</v>
       </c>
@@ -5164,7 +5341,7 @@
         <v>71.400000000000475</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51">
       <c r="A51">
         <v>111.40000000000104</v>
       </c>
@@ -5184,7 +5361,7 @@
         <v>22.199999999999953</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52">
       <c r="A52">
         <v>113.20000000000107</v>
       </c>
@@ -5204,7 +5381,7 @@
         <v>18.799999999999965</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53">
       <c r="A53">
         <v>84.400000000000659</v>
       </c>
@@ -5224,7 +5401,7 @@
         <v>21.799999999999955</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54">
       <c r="A54">
         <v>84.400000000000659</v>
       </c>
@@ -5244,7 +5421,7 @@
         <v>26.999999999999936</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55">
       <c r="A55">
         <v>111.40000000000104</v>
       </c>
@@ -5264,7 +5441,7 @@
         <v>21.199999999999957</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56">
       <c r="A56">
         <v>92.600000000000776</v>
       </c>
@@ -5284,7 +5461,7 @@
         <v>23.399999999999949</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57">
       <c r="A57">
         <v>64.200000000000372</v>
       </c>
@@ -5304,7 +5481,7 @@
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58">
       <c r="A58">
         <v>66.000000000000398</v>
       </c>
@@ -5324,7 +5501,7 @@
         <v>8.6000000000000014</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59">
       <c r="A59">
         <v>68.000000000000426</v>
       </c>
@@ -5344,7 +5521,7 @@
         <v>8.6000000000000014</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60">
       <c r="A60">
         <v>107.60000000000099</v>
       </c>
@@ -5364,7 +5541,7 @@
         <v>18.599999999999966</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61">
       <c r="A61">
         <v>79.000000000000583</v>
       </c>
@@ -5384,7 +5561,7 @@
         <v>17.39999999999997</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62">
       <c r="A62">
         <v>82.400000000000631</v>
       </c>
@@ -5404,7 +5581,7 @@
         <v>5.4000000000000021</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63">
       <c r="A63">
         <v>82.800000000000637</v>
       </c>
@@ -5424,7 +5601,7 @@
         <v>32.599999999999923</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64">
       <c r="A64">
         <v>107.80000000000099</v>
       </c>
@@ -5444,7 +5621,7 @@
         <v>20.399999999999959</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65">
       <c r="A65">
         <v>76.200000000000543</v>
       </c>
@@ -5464,7 +5641,7 @@
         <v>12.199999999999989</v>
       </c>
     </row>
-    <row r="66" spans="1:6">
+    <row r="66">
       <c r="A66">
         <v>85.600000000000676</v>
       </c>
@@ -5484,7 +5661,7 @@
         <v>18.199999999999967</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67">
       <c r="A67">
         <v>102.40000000000092</v>
       </c>
@@ -5504,7 +5681,7 @@
         <v>19.399999999999963</v>
       </c>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68">
       <c r="A68">
         <v>101.80000000000091</v>
       </c>
@@ -5524,7 +5701,7 @@
         <v>20.999999999999957</v>
       </c>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69">
       <c r="A69">
         <v>103.80000000000094</v>
       </c>
@@ -5544,7 +5721,7 @@
         <v>18.199999999999967</v>
       </c>
     </row>
-    <row r="70" spans="1:6">
+    <row r="70">
       <c r="A70">
         <v>73.000000000000497</v>
       </c>
@@ -5564,7 +5741,7 @@
         <v>42.20000000000006</v>
       </c>
     </row>
-    <row r="71" spans="1:6">
+    <row r="71">
       <c r="A71">
         <v>68.600000000000435</v>
       </c>
@@ -5584,7 +5761,7 @@
         <v>27.399999999999935</v>
       </c>
     </row>
-    <row r="72" spans="1:6">
+    <row r="72">
       <c r="A72">
         <v>72.000000000000483</v>
       </c>
@@ -5604,7 +5781,7 @@
         <v>9.9999999999999964</v>
       </c>
     </row>
-    <row r="73" spans="1:6">
+    <row r="73">
       <c r="A73">
         <v>77.40000000000056</v>
       </c>
@@ -5624,7 +5801,7 @@
         <v>17.199999999999971</v>
       </c>
     </row>
-    <row r="74" spans="1:6">
+    <row r="74">
       <c r="A74">
         <v>75.800000000000537</v>
       </c>
@@ -5644,7 +5821,7 @@
         <v>46.600000000000122</v>
       </c>
     </row>
-    <row r="75" spans="1:6">
+    <row r="75">
       <c r="A75">
         <v>98.200000000000855</v>
       </c>
@@ -5664,7 +5841,7 @@
         <v>26.399999999999938</v>
       </c>
     </row>
-    <row r="76" spans="1:6">
+    <row r="76">
       <c r="A76">
         <v>90.80000000000075</v>
       </c>
@@ -5684,7 +5861,7 @@
         <v>8.0000000000000036</v>
       </c>
     </row>
-    <row r="77" spans="1:6">
+    <row r="77">
       <c r="A77">
         <v>61.600000000000335</v>
       </c>
@@ -5704,7 +5881,7 @@
         <v>17.39999999999997</v>
       </c>
     </row>
-    <row r="78" spans="1:6">
+    <row r="78">
       <c r="A78">
         <v>70.600000000000463</v>
       </c>
@@ -5724,7 +5901,7 @@
         <v>44.400000000000091</v>
       </c>
     </row>
-    <row r="79" spans="1:6">
+    <row r="79">
       <c r="A79">
         <v>72.600000000000492</v>
       </c>
@@ -5744,7 +5921,7 @@
         <v>19.399999999999963</v>
       </c>
     </row>
-    <row r="80" spans="1:6">
+    <row r="80">
       <c r="A80">
         <v>60.600000000000321</v>
       </c>
@@ -5764,7 +5941,7 @@
         <v>19.399999999999963</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81">
       <c r="A81">
         <v>89.800000000000736</v>
       </c>
@@ -5784,7 +5961,7 @@
         <v>17.39999999999997</v>
       </c>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82">
       <c r="A82">
         <v>87.400000000000702</v>
       </c>
@@ -5804,7 +5981,7 @@
         <v>10.799999999999994</v>
       </c>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83">
       <c r="A83">
         <v>79.200000000000585</v>
       </c>
@@ -5824,7 +6001,7 @@
         <v>28.79999999999993</v>
       </c>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84">
       <c r="A84">
         <v>81.400000000000617</v>
       </c>
@@ -5844,7 +6021,7 @@
         <v>28.79999999999993</v>
       </c>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85">
       <c r="A85">
         <v>84.400000000000659</v>
       </c>
@@ -5864,7 +6041,7 @@
         <v>20.399999999999959</v>
       </c>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86">
       <c r="A86">
         <v>85.800000000000679</v>
       </c>
@@ -5884,7 +6061,7 @@
         <v>26.599999999999937</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87">
       <c r="A87">
         <v>103.60000000000093</v>
       </c>
@@ -5904,7 +6081,7 @@
         <v>65.600000000000392</v>
       </c>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88">
       <c r="A88">
         <v>71.200000000000472</v>
       </c>
@@ -5924,7 +6101,7 @@
         <v>53.600000000000222</v>
       </c>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89">
       <c r="A89">
         <v>63.000000000000355</v>
       </c>
@@ -5944,7 +6121,7 @@
         <v>11.999999999999989</v>
       </c>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90">
       <c r="A90">
         <v>96.200000000000827</v>
       </c>
@@ -5964,7 +6141,7 @@
         <v>20.399999999999959</v>
       </c>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91">
       <c r="B91" s="1">
         <f>AVERAGE(B1:B90)</f>
         <v>23.380000000000013</v>
@@ -5986,7 +6163,7 @@
         <v>26.266666666666673</v>
       </c>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92">
       <c r="B92" s="1">
         <f>MIN(B1:B90)</f>
         <v>0.2</v>
@@ -6008,7 +6185,7 @@
         <v>5.4000000000000021</v>
       </c>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93">
       <c r="B93" s="1">
         <f>MAX(B1:B90)</f>
         <v>67.600000000000421</v>
@@ -6031,8 +6208,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:F91">
-    <sortCondition descending="1" ref="D1:D91"/>
+  <sortState ref="A1:F91">
+    <sortCondition descending="true" ref="D1:D91"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>